<commit_message>
Got rid of pandas Panel objects, replaced with HDFContainers. Cleaned up import paths in tests. Moved binaries to bin folder.
</commit_message>
<xml_diff>
--- a/losspager/data/pager_regions.xlsx
+++ b/losspager/data/pager_regions.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10123"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhearne/src/python/losspager/losspager/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FDA5E8-8A7C-4443-9A46-4F7190E31056}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="1720" windowWidth="33580" windowHeight="16740" activeTab="1"/>
+    <workbookView xWindow="1320" yWindow="1720" windowWidth="32280" windowHeight="16740" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
     <sheet name="Region5" sheetId="5" r:id="rId5"/>
     <sheet name="Region6" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1031,9 +1037,6 @@
     <t>Congo</t>
   </si>
   <si>
-    <t>C√¥te d'Ivoire</t>
-  </si>
-  <si>
     <t>Cook Islands</t>
   </si>
   <si>
@@ -1557,12 +1560,15 @@
   </si>
   <si>
     <t>Overall, the population in this region resides in structures that are vulnerable to earthquake shaking, though resistant structures exist.</t>
+  </si>
+  <si>
+    <t>Côte d'Ivoire</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1890,6 +1896,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2177,19 +2191,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="110.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2197,10 +2211,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2208,10 +2222,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -2219,7 +2233,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2239,20 +2253,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="106" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2260,10 +2274,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2271,10 +2285,10 @@
         <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2282,7 +2296,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2290,15 +2304,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>487</v>
+      </c>
+      <c r="B5" t="s">
         <v>488</v>
       </c>
-      <c r="B5" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2306,15 +2320,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>497</v>
+      </c>
+      <c r="B7" t="s">
         <v>498</v>
       </c>
-      <c r="B7" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2322,15 +2336,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>491</v>
+      </c>
+      <c r="B9" t="s">
         <v>492</v>
       </c>
-      <c r="B9" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2338,7 +2352,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2346,7 +2360,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2354,15 +2368,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>493</v>
+      </c>
+      <c r="B13" t="s">
         <v>494</v>
       </c>
-      <c r="B13" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2370,7 +2384,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2378,7 +2392,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2386,7 +2400,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -2394,7 +2408,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2402,7 +2416,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2410,7 +2424,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2418,7 +2432,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2426,7 +2440,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2434,7 +2448,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2442,7 +2456,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2450,7 +2464,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2458,7 +2472,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2466,7 +2480,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2474,7 +2488,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2482,7 +2496,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2490,15 +2504,15 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>499</v>
+      </c>
+      <c r="B30" t="s">
         <v>500</v>
       </c>
-      <c r="B30" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2506,7 +2520,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2514,7 +2528,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -2522,7 +2536,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2530,7 +2544,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2538,15 +2552,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>501</v>
+      </c>
+      <c r="B36" t="s">
         <v>502</v>
       </c>
-      <c r="B36" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -2554,7 +2568,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -2562,7 +2576,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -2570,7 +2584,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -2578,7 +2592,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -2586,7 +2600,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>111</v>
       </c>
@@ -2594,7 +2608,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>117</v>
       </c>
@@ -2602,7 +2616,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>116</v>
       </c>
@@ -2610,12 +2624,12 @@
         <v>167</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>489</v>
+      </c>
+      <c r="B45" t="s">
         <v>490</v>
-      </c>
-      <c r="B45" t="s">
-        <v>491</v>
       </c>
     </row>
   </sheetData>
@@ -2630,20 +2644,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="94.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2651,10 +2665,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -2662,10 +2676,10 @@
         <v>127</v>
       </c>
       <c r="C2" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -2673,7 +2687,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -2681,7 +2695,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -2689,7 +2703,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -2697,7 +2711,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -2705,7 +2719,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>82</v>
       </c>
@@ -2713,7 +2727,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -2721,7 +2735,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -2729,7 +2743,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -2737,7 +2751,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -2745,7 +2759,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>87</v>
       </c>
@@ -2753,7 +2767,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>88</v>
       </c>
@@ -2761,7 +2775,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>89</v>
       </c>
@@ -2769,7 +2783,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>90</v>
       </c>
@@ -2777,7 +2791,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>91</v>
       </c>
@@ -2785,7 +2799,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>92</v>
       </c>
@@ -2793,7 +2807,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>93</v>
       </c>
@@ -2801,7 +2815,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>94</v>
       </c>
@@ -2809,7 +2823,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>95</v>
       </c>
@@ -2817,7 +2831,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>96</v>
       </c>
@@ -2825,7 +2839,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>97</v>
       </c>
@@ -2833,7 +2847,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>98</v>
       </c>
@@ -2841,7 +2855,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>99</v>
       </c>
@@ -2849,7 +2863,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>100</v>
       </c>
@@ -2857,7 +2871,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>101</v>
       </c>
@@ -2865,7 +2879,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -2873,7 +2887,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>103</v>
       </c>
@@ -2881,7 +2895,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>104</v>
       </c>
@@ -2889,7 +2903,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>105</v>
       </c>
@@ -2897,7 +2911,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>108</v>
       </c>
@@ -2905,7 +2919,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>109</v>
       </c>
@@ -2913,7 +2927,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>110</v>
       </c>
@@ -2921,7 +2935,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>112</v>
       </c>
@@ -2929,7 +2943,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>113</v>
       </c>
@@ -2937,7 +2951,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>114</v>
       </c>
@@ -2945,7 +2959,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>115</v>
       </c>
@@ -2953,7 +2967,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>118</v>
       </c>
@@ -2961,7 +2975,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>119</v>
       </c>
@@ -2969,7 +2983,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>120</v>
       </c>
@@ -2977,7 +2991,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>121</v>
       </c>
@@ -2985,7 +2999,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>122</v>
       </c>
@@ -2993,7 +3007,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>123</v>
       </c>
@@ -3001,7 +3015,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>124</v>
       </c>
@@ -3009,7 +3023,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>125</v>
       </c>
@@ -3017,7 +3031,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>126</v>
       </c>
@@ -3025,188 +3039,188 @@
         <v>177</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>239</v>
       </c>
       <c r="B48" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>220</v>
       </c>
       <c r="B49" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>221</v>
       </c>
       <c r="B50" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>223</v>
       </c>
       <c r="B51" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>211</v>
       </c>
       <c r="B52" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>212</v>
       </c>
       <c r="B53" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>201</v>
       </c>
       <c r="B54" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>202</v>
       </c>
       <c r="B55" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>225</v>
       </c>
       <c r="B56" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>228</v>
       </c>
       <c r="B57" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>237</v>
       </c>
       <c r="B58" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>251</v>
       </c>
       <c r="B59" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>269</v>
       </c>
       <c r="B60" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>271</v>
       </c>
       <c r="B61" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>272</v>
       </c>
       <c r="B62" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>273</v>
       </c>
       <c r="B63" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>274</v>
       </c>
       <c r="B64" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>275</v>
       </c>
       <c r="B65" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>276</v>
       </c>
       <c r="B66" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>279</v>
       </c>
       <c r="B67" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>281</v>
       </c>
       <c r="B68" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>250</v>
       </c>
       <c r="B69" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>256</v>
       </c>
       <c r="B70" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -3221,20 +3235,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="106" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3242,10 +3256,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>178</v>
       </c>
@@ -3253,10 +3267,10 @@
         <v>317</v>
       </c>
       <c r="C2" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>179</v>
       </c>
@@ -3264,7 +3278,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>180</v>
       </c>
@@ -3272,7 +3286,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -3280,7 +3294,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>182</v>
       </c>
@@ -3288,7 +3302,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>183</v>
       </c>
@@ -3296,7 +3310,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>184</v>
       </c>
@@ -3304,7 +3318,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>185</v>
       </c>
@@ -3312,7 +3326,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>186</v>
       </c>
@@ -3320,7 +3334,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>187</v>
       </c>
@@ -3328,7 +3342,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>188</v>
       </c>
@@ -3336,7 +3350,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>189</v>
       </c>
@@ -3344,7 +3358,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>190</v>
       </c>
@@ -3352,7 +3366,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>191</v>
       </c>
@@ -3360,7 +3374,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>192</v>
       </c>
@@ -3368,543 +3382,543 @@
         <v>331</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>196</v>
       </c>
       <c r="B17" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>197</v>
       </c>
       <c r="B18" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>199</v>
       </c>
       <c r="B19" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>200</v>
       </c>
       <c r="B20" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>203</v>
       </c>
       <c r="B21" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>204</v>
       </c>
       <c r="B22" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>205</v>
       </c>
       <c r="B23" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B24" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B25" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>210</v>
       </c>
       <c r="B26" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>213</v>
       </c>
       <c r="B27" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>214</v>
       </c>
       <c r="B28" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>215</v>
       </c>
       <c r="B29" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>217</v>
       </c>
       <c r="B30" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>218</v>
       </c>
       <c r="B31" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>219</v>
       </c>
       <c r="B32" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>224</v>
       </c>
       <c r="B33" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>226</v>
       </c>
       <c r="B34" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>227</v>
       </c>
       <c r="B35" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>230</v>
       </c>
       <c r="B36" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>296</v>
       </c>
       <c r="B37" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>307</v>
       </c>
       <c r="B38" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>233</v>
       </c>
       <c r="B39" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>299</v>
       </c>
       <c r="B40" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>234</v>
       </c>
       <c r="B41" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>235</v>
       </c>
       <c r="B42" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>236</v>
       </c>
       <c r="B43" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>238</v>
       </c>
       <c r="B44" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>240</v>
       </c>
       <c r="B45" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>241</v>
       </c>
       <c r="B46" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>242</v>
       </c>
       <c r="B47" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>243</v>
       </c>
       <c r="B48" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>245</v>
       </c>
       <c r="B49" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>246</v>
       </c>
       <c r="B50" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>248</v>
       </c>
       <c r="B51" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>249</v>
       </c>
       <c r="B52" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>252</v>
       </c>
       <c r="B53" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>253</v>
       </c>
       <c r="B54" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>254</v>
       </c>
       <c r="B55" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>255</v>
       </c>
       <c r="B56" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>257</v>
       </c>
       <c r="B57" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>258</v>
       </c>
       <c r="B58" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>259</v>
       </c>
       <c r="B59" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>263</v>
       </c>
       <c r="B60" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>266</v>
       </c>
       <c r="B61" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>267</v>
       </c>
       <c r="B62" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>268</v>
       </c>
       <c r="B63" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>277</v>
       </c>
       <c r="B64" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>280</v>
       </c>
       <c r="B65" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>283</v>
       </c>
       <c r="B66" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>287</v>
       </c>
       <c r="B67" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>290</v>
       </c>
       <c r="B68" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>291</v>
       </c>
       <c r="B69" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>292</v>
       </c>
       <c r="B70" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>293</v>
       </c>
       <c r="B71" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>294</v>
       </c>
       <c r="B72" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>295</v>
       </c>
       <c r="B73" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>297</v>
       </c>
       <c r="B74" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>298</v>
       </c>
       <c r="B75" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>302</v>
       </c>
       <c r="B76" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>306</v>
       </c>
       <c r="B77" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>308</v>
       </c>
       <c r="B78" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>309</v>
       </c>
       <c r="B79" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>312</v>
       </c>
       <c r="B80" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>313</v>
       </c>
       <c r="B81" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>314</v>
       </c>
       <c r="B82" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>316</v>
       </c>
       <c r="B83" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>106</v>
       </c>
@@ -3912,7 +3926,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>107</v>
       </c>
@@ -3920,12 +3934,12 @@
         <v>158</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>495</v>
+      </c>
+      <c r="B86" t="s">
         <v>496</v>
-      </c>
-      <c r="B86" t="s">
-        <v>497</v>
       </c>
     </row>
   </sheetData>
@@ -3940,20 +3954,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="110.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3961,261 +3975,261 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>456</v>
+      </c>
+      <c r="B2" t="s">
+        <v>470</v>
+      </c>
+      <c r="C2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>457</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>471</v>
       </c>
-      <c r="C2" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>458</v>
-      </c>
-      <c r="B3" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>222</v>
       </c>
       <c r="B4" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>264</v>
       </c>
       <c r="B5" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>464</v>
+      </c>
+      <c r="B6" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>465</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>466</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>467</v>
-      </c>
-      <c r="B8" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B9" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>206</v>
       </c>
       <c r="B10" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>207</v>
       </c>
       <c r="B11" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>216</v>
       </c>
       <c r="B12" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>231</v>
       </c>
       <c r="B13" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>232</v>
       </c>
       <c r="B14" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>244</v>
       </c>
       <c r="B15" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>270</v>
       </c>
       <c r="B16" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>284</v>
       </c>
       <c r="B17" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>285</v>
       </c>
       <c r="B18" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>286</v>
       </c>
       <c r="B19" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>288</v>
       </c>
       <c r="B20" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>289</v>
       </c>
       <c r="B21" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>300</v>
       </c>
       <c r="B22" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>301</v>
       </c>
       <c r="B23" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>229</v>
       </c>
       <c r="B24" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>247</v>
       </c>
       <c r="B25" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>315</v>
       </c>
       <c r="B26" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>310</v>
       </c>
       <c r="B27" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>311</v>
       </c>
       <c r="B28" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>303</v>
       </c>
       <c r="B29" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>304</v>
       </c>
       <c r="B30" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>305</v>
       </c>
       <c r="B31" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>278</v>
       </c>
       <c r="B32" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>193</v>
       </c>
@@ -4223,7 +4237,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>194</v>
       </c>
@@ -4231,7 +4245,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>195</v>
       </c>
@@ -4239,76 +4253,76 @@
         <v>334</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>208</v>
       </c>
       <c r="B36" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>209</v>
       </c>
       <c r="B37" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>198</v>
       </c>
       <c r="B38" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>265</v>
       </c>
       <c r="B39" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>260</v>
       </c>
       <c r="B40" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>261</v>
       </c>
       <c r="B41" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>262</v>
       </c>
       <c r="B42" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>505</v>
+      </c>
+      <c r="B43" t="s">
         <v>506</v>
       </c>
-      <c r="B43" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B44" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
   </sheetData>
@@ -4323,20 +4337,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="110.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4344,66 +4358,66 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C2" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>503</v>
+      </c>
+      <c r="B3" t="s">
         <v>504</v>
       </c>
-      <c r="B3" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B4" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>459</v>
+      </c>
+      <c r="B5" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>460</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>461</v>
-      </c>
-      <c r="B6" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B7" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>282</v>
       </c>
       <c r="B8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>

</xml_diff>